<commit_message>
Correction coquille sur profils 0052e560bf73743150ec7554e09d70e5a0f5c65d
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/StructureDefinition-fr-medication-compound2.xlsx
+++ b/FinalisationMappingPosologie/ig/StructureDefinition-fr-medication-compound2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="281">
   <si>
     <t>Property</t>
   </si>
@@ -42,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>French compound Medication</t>
+    <t>French compound Medication 2</t>
   </si>
   <si>
     <t>Status</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-01-20T09:27:26+00:00</t>
+    <t>2025-01-20T09:49:22+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -685,10 +685,10 @@
     <t>When Medication is referenced from MedicationRequest, this is the ordered form.  When Medication is referenced within MedicationDispense, this is the dispensed form.  When Medication is referenced within MedicationAdministration, this is administered form.</t>
   </si>
   <si>
-    <t>extensible</t>
-  </si>
-  <si>
-    <t>https://hl7.fr/fhir/fr/medication/ValueSet/fr-mp-dose-form</t>
+    <t>A coded concept defining the form of a medication.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/medication-form-codes</t>
   </si>
   <si>
     <t>coding.code =  //element(*,DrugCodedType)/FormCode@@ -1242,7 +1242,7 @@
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="55.39453125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="53.41796875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="48.0390625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
@@ -3381,9 +3381,11 @@
         <v>21</v>
       </c>
       <c r="X19" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="Y19" t="s" s="2">
         <v>213</v>
       </c>
-      <c r="Y19" s="2"/>
       <c r="Z19" t="s" s="2">
         <v>214</v>
       </c>

</xml_diff>